<commit_message>
typos fixed. user documentation updated
</commit_message>
<xml_diff>
--- a/doc/projectFiles/SprintBacklog.xlsx
+++ b/doc/projectFiles/SprintBacklog.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="655" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="655" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -202,9 +201,6 @@
     <t>3-2</t>
   </si>
   <si>
-    <t>Als &lt;MM&gt; will ich das Tweets nach Anlegen einer Veranstaltung zur Verfügung haben, so dass ich später eine Sentimentanalyse fahren kann</t>
-  </si>
-  <si>
     <t>CronJob/Scheduled Task für die SammelApp anlegen</t>
   </si>
   <si>
@@ -248,38 +244,22 @@
   </si>
   <si>
     <t>User Manual</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich, dass Tweets nach Anlegen einer Veranstaltung zur Verfügung haben, so dass ich später eine Sentimentanalyse fahren kann</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="14"/>
@@ -289,7 +269,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -297,7 +277,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -314,7 +294,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -322,92 +302,330 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="109.433198380567"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.53441295546559"/>
+    <col min="1" max="1" width="12.140625"/>
+    <col min="2" max="2" width="109.42578125"/>
+    <col min="3" max="4" width="11.28515625"/>
+    <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,11 +638,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -438,7 +656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" ht="18.75">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -448,35 +666,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="1">
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="1">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -486,7 +704,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -496,7 +714,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -506,7 +724,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" ht="18.75">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>20</v>
@@ -514,7 +732,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" ht="18.75">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -522,7 +740,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" ht="18.75">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -530,7 +748,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -540,7 +758,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -550,7 +768,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -560,13 +778,13 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" ht="18.75">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" ht="18.75">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>29</v>
@@ -576,7 +794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -586,7 +804,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4" ht="18.75">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>31</v>
@@ -594,7 +812,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4" ht="18.75">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>32</v>
@@ -602,7 +820,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4" ht="18.75">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>33</v>
@@ -610,7 +828,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:4" ht="18.75">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>24</v>
@@ -618,7 +836,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4" ht="18.75">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -628,7 +846,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:4" ht="18.75">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -638,13 +856,13 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:4" ht="18.75">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:4" ht="18.75">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
         <v>34</v>
@@ -654,13 +872,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:4" ht="18.75">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:4" ht="18.75">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -670,7 +888,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:4" ht="18.75">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -680,7 +898,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:4" ht="18.75">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -690,7 +908,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:4" ht="18.75">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -700,7 +918,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:4" ht="18.75">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -709,39 +927,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E65536"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="121.935222672065"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8663967611336"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.7246963562753"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8987854251012"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col min="1" max="1" width="18"/>
+    <col min="2" max="2" width="12.28515625"/>
+    <col min="3" max="3" width="122"/>
+    <col min="4" max="4" width="23.85546875"/>
+    <col min="5" max="5" width="8.7109375"/>
+    <col min="6" max="6" width="11.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -758,7 +967,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -769,7 +978,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -780,7 +989,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -791,7 +1000,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -802,7 +1011,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -811,15 +1020,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="true" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>47</v>
       </c>
@@ -827,12 +1036,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="true" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" s="3" customFormat="1">
       <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" s="4" customFormat="true" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -843,7 +1052,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
@@ -851,7 +1060,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3">
       <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
@@ -859,7 +1068,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
         <v>44</v>
       </c>
@@ -867,7 +1076,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:3">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
@@ -875,7 +1084,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
@@ -883,7 +1092,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
         <v>11</v>
       </c>
@@ -891,7 +1100,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:3">
       <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
@@ -899,7 +1108,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
@@ -907,172 +1116,150 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:3" ht="12.4" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
+    <row r="27" spans="1:3" s="3" customFormat="1">
+      <c r="A27"/>
       <c r="B27" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="3" customFormat="1">
+      <c r="A37"/>
+      <c r="B37" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="0" t="s">
+      <c r="C44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="0" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new backlogs checked in
</commit_message>
<xml_diff>
--- a/doc/projectFiles/SprintBacklog.xlsx
+++ b/doc/projectFiles/SprintBacklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="655" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="655" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="90">
   <si>
     <t>Spalte1</t>
   </si>
@@ -247,6 +247,45 @@
   </si>
   <si>
     <t>Als &lt;MM&gt; will ich, dass Tweets nach Anlegen einer Veranstaltung zur Verfügung haben, so dass ich später eine Sentimentanalyse fahren kann</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich eine positiv/negativ Sentiment Analyse der Tweets erhalten</t>
+  </si>
+  <si>
+    <t>4-1</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich die vorhandenen Tweets einschränken, sodass nur relevante Tweets analysiert werden</t>
+  </si>
+  <si>
+    <t>userstory ID</t>
+  </si>
+  <si>
+    <t>Johannes/Manfred</t>
+  </si>
+  <si>
+    <t>Modelklasse</t>
+  </si>
+  <si>
+    <t>Datenbank</t>
+  </si>
+  <si>
+    <t>Controllerklasse</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Paging/Springer</t>
+  </si>
+  <si>
+    <t>Alle</t>
+  </si>
+  <si>
+    <t>Defect Liste</t>
   </si>
 </sst>
 </file>
@@ -936,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1250,15 +1289,220 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="1025" width="8.5703125"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>